<commit_message>
Master through X Y and EUCL
</commit_message>
<xml_diff>
--- a/LOCOMOTION-MASTER-CM.xlsx
+++ b/LOCOMOTION-MASTER-CM.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="15940" tabRatio="500" firstSheet="3" activeTab="4"/>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15980" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="15940" tabRatio="500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER-ABC" sheetId="1" r:id="rId1"/>
@@ -12589,8 +12589,8 @@
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H161" sqref="H161"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="92" workbookViewId="1">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="92" workbookViewId="1">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>